<commit_message>
lanjutan untuk no 2
jawaban no 2
</commit_message>
<xml_diff>
--- a/laporan_pengamatan.xlsx
+++ b/laporan_pengamatan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="57">
   <si>
     <t>col_0</t>
   </si>
@@ -176,6 +176,21 @@
   </si>
   <si>
     <t>esr</t>
+  </si>
+  <si>
+    <t>dana pensi</t>
+  </si>
+  <si>
+    <t>inflasi</t>
+  </si>
+  <si>
+    <t>gaji sisa</t>
+  </si>
+  <si>
+    <t>duit awal</t>
+  </si>
+  <si>
+    <t>total dana pensi</t>
   </si>
 </sst>
 </file>
@@ -644,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection sqref="A1:Z17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2014,10 +2029,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO39"/>
+  <dimension ref="A1:AP44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="AH19" workbookViewId="0">
+      <selection activeCell="AN28" sqref="AN28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2025,6 +2040,7 @@
     <col min="31" max="33" width="12" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="11" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="16.77734375" customWidth="1"/>
+    <col min="42" max="42" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -3404,7 +3420,7 @@
         <v>6.3220816406250012E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:41">
+    <row r="17" spans="1:42">
       <c r="AA17" s="2"/>
       <c r="AC17" t="s">
         <v>42</v>
@@ -3425,7 +3441,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:41">
+    <row r="18" spans="1:42">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -3541,7 +3557,7 @@
         <v>0.90457077438496636</v>
       </c>
     </row>
-    <row r="19" spans="1:41">
+    <row r="19" spans="1:42">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -3641,7 +3657,7 @@
         <v>2.9762397024305547E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:41">
+    <row r="20" spans="1:42">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -3741,10 +3757,13 @@
         <v>1.2794223796874999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:41">
+    <row r="21" spans="1:42">
       <c r="AA21" s="2"/>
-    </row>
-    <row r="22" spans="1:41">
+      <c r="AP21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -3844,18 +3863,25 @@
       <c r="AI22" t="s">
         <v>47</v>
       </c>
+      <c r="AK22" t="s">
+        <v>53</v>
+      </c>
       <c r="AL22">
         <v>1</v>
       </c>
       <c r="AM22">
-        <f>AI24*(SUM(AL22:AL38))</f>
-        <v>1982149392.4728963</v>
+        <f>AP22*(SUM(AL22:AL41))</f>
+        <v>1790012671.8180029</v>
       </c>
       <c r="AO22" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:41">
+      <c r="AP22">
+        <f>(AC23+1)*60000000</f>
+        <v>70073856.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -3944,15 +3970,15 @@
       </c>
       <c r="AC23">
         <f>SUM(AB23:AB38)</f>
-        <v>0.167893025</v>
+        <v>0.16789760833333334</v>
       </c>
       <c r="AD23">
         <f>Z23-AC23</f>
-        <v>-0.150755525</v>
+        <v>-0.15076010833333334</v>
       </c>
       <c r="AE23">
         <f>AD23*AD23</f>
-        <v>2.2727228318025625E-2</v>
+        <v>2.2728610264678404E-2</v>
       </c>
       <c r="AF23">
         <f>AE23*AA23</f>
@@ -3960,15 +3986,15 @@
       </c>
       <c r="AG23">
         <f>SUM(AF23:AF38)</f>
-        <v>3.9999206133993041E-2</v>
+        <v>3.9999262997187486E-2</v>
       </c>
       <c r="AH23">
         <f>SQRT(AG23)</f>
-        <v>0.19999801532513528</v>
+        <v>0.19999815748448155</v>
       </c>
       <c r="AI23">
         <f>AH23/AC23</f>
-        <v>1.191222895204463</v>
+        <v>1.1911912234474347</v>
       </c>
       <c r="AJ23">
         <v>1</v>
@@ -3977,19 +4003,23 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL23">
-        <f>1*AK23</f>
+        <f>AL22*AK23</f>
         <v>1.0249999999999999</v>
       </c>
       <c r="AN23">
         <f>AC23-0.025</f>
-        <v>0.14289302500000001</v>
+        <v>0.14289760833333334</v>
       </c>
       <c r="AO23">
         <f>AN23/AH23</f>
-        <v>0.71447221497523306</v>
-      </c>
-    </row>
-    <row r="24" spans="1:41">
+        <v>0.71449462400382957</v>
+      </c>
+      <c r="AP23">
+        <f>(AI24*AK23)+60000000</f>
+        <v>941499999.99999988</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -4089,14 +4119,14 @@
         <v>3.7190539609374992E-3</v>
       </c>
       <c r="AG24" s="2">
-        <v>100000000</v>
+        <v>800000000</v>
       </c>
       <c r="AH24">
-        <v>5000000</v>
+        <v>60000000</v>
       </c>
       <c r="AI24">
-        <f>AG24-AH24</f>
-        <v>95000000</v>
+        <f>AG24+AH24</f>
+        <v>860000000</v>
       </c>
       <c r="AJ24">
         <v>2</v>
@@ -4105,11 +4135,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL24">
-        <f>AL23*AK24</f>
+        <f t="shared" ref="AL24:AL42" si="12">AL23*AK24</f>
         <v>1.0506249999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:41">
+      <c r="AP24">
+        <f>(AI25*AK24)+60000000</f>
+        <v>1025037499.9999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -4208,6 +4242,15 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="AG25" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH25">
+        <v>60000000</v>
+      </c>
+      <c r="AI25">
+        <v>941500000</v>
+      </c>
       <c r="AJ25">
         <v>3</v>
       </c>
@@ -4215,11 +4258,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL25">
-        <f>AL24*AK25</f>
+        <f t="shared" si="12"/>
         <v>1.0768906249999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:41">
+      <c r="AP25">
+        <f>(AI26*AK25)+60000000</f>
+        <v>1110663437.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:42">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -4311,13 +4358,19 @@
         <v>5.0287500000000006E-2</v>
       </c>
       <c r="AE26">
-        <f t="shared" ref="AE26:AE38" si="12">AD26*AD26</f>
+        <f t="shared" ref="AE26:AE38" si="13">AD26*AD26</f>
         <v>2.5288326562500005E-3</v>
       </c>
       <c r="AF26">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="AH26">
+        <v>60000000</v>
+      </c>
+      <c r="AI26">
+        <v>1025037500</v>
+      </c>
       <c r="AJ26">
         <v>4</v>
       </c>
@@ -4325,11 +4378,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL26">
-        <f t="shared" ref="AL26:AL38" si="13">AL25*AK26</f>
+        <f t="shared" si="12"/>
         <v>1.1038128906249998</v>
       </c>
-    </row>
-    <row r="27" spans="1:41">
+      <c r="AP26">
+        <f>(AI27*AK26)+60000000</f>
+        <v>1198430023.9499998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -4410,23 +4467,29 @@
         <v>4.1166666666666678E-3</v>
       </c>
       <c r="AA27" s="2">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="AB27">
         <f t="shared" si="9"/>
-        <v>4.116666666666668E-5</v>
+        <v>0</v>
       </c>
       <c r="AD27">
         <f t="shared" si="10"/>
         <v>4.1166666666666678E-3</v>
       </c>
       <c r="AE27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.6946944444444454E-5</v>
       </c>
       <c r="AF27">
         <f t="shared" si="11"/>
-        <v>1.6946944444444456E-7</v>
+        <v>0</v>
+      </c>
+      <c r="AH27">
+        <v>60000000</v>
+      </c>
+      <c r="AI27">
+        <v>1110663438</v>
       </c>
       <c r="AJ27">
         <v>5</v>
@@ -4435,11 +4498,18 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.1314082128906247</v>
       </c>
-    </row>
-    <row r="28" spans="1:41">
+      <c r="AM27" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP27">
+        <f>(AI28*AK27)+60000000</f>
+        <v>1288390774.5999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -4520,23 +4590,29 @@
         <v>4.358333333333333E-3</v>
       </c>
       <c r="AA28" s="2">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AB28">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4.3583333333333333E-5</v>
       </c>
       <c r="AD28">
         <f t="shared" si="10"/>
         <v>4.358333333333333E-3</v>
       </c>
       <c r="AE28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.8995069444444441E-5</v>
       </c>
       <c r="AF28">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.8995069444444441E-7</v>
+      </c>
+      <c r="AH28">
+        <v>60000000</v>
+      </c>
+      <c r="AI28">
+        <v>1198430024</v>
       </c>
       <c r="AJ28">
         <v>6</v>
@@ -4545,11 +4621,19 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.1596934182128902</v>
       </c>
-    </row>
-    <row r="29" spans="1:41">
+      <c r="AM28">
+        <f>AM22+AP41</f>
+        <v>4601612277.3180027</v>
+      </c>
+      <c r="AP28">
+        <f>(AI29*AK28)+60000000</f>
+        <v>1380600544.375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -4630,23 +4714,29 @@
         <v>8.287499999999998E-3</v>
       </c>
       <c r="AA29" s="2">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="AB29">
         <f t="shared" si="9"/>
-        <v>8.2874999999999982E-5</v>
+        <v>0</v>
       </c>
       <c r="AD29">
         <f t="shared" si="10"/>
         <v>8.287499999999998E-3</v>
       </c>
       <c r="AE29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6.868265624999997E-5</v>
       </c>
       <c r="AF29">
         <f t="shared" si="11"/>
-        <v>6.8682656249999967E-7</v>
+        <v>0</v>
+      </c>
+      <c r="AH29">
+        <v>60000000</v>
+      </c>
+      <c r="AI29">
+        <v>1288390775</v>
       </c>
       <c r="AJ29">
         <v>7</v>
@@ -4655,11 +4745,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.1886857536682123</v>
       </c>
-    </row>
-    <row r="30" spans="1:41">
+      <c r="AP29">
+        <f>(AI30*AK29)+60000000</f>
+        <v>1475115557.5999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:42">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -4740,23 +4834,29 @@
         <v>8.5041666666666668E-3</v>
       </c>
       <c r="AA30" s="2">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AB30">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>8.5041666666666669E-5</v>
       </c>
       <c r="AD30">
         <f t="shared" si="10"/>
         <v>8.5041666666666668E-3</v>
       </c>
       <c r="AE30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7.2320850694444452E-5</v>
       </c>
       <c r="AF30">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>7.2320850694444455E-7</v>
+      </c>
+      <c r="AH30">
+        <v>60000000</v>
+      </c>
+      <c r="AI30">
+        <v>1380600544</v>
       </c>
       <c r="AJ30">
         <v>8</v>
@@ -4765,11 +4865,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.2184028975099175</v>
       </c>
-    </row>
-    <row r="31" spans="1:41">
+      <c r="AP30">
+        <f>(AI31*AK30)+60000000</f>
+        <v>1571993446.9499998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -4861,13 +4965,19 @@
         <v>1.2866666666666665E-2</v>
       </c>
       <c r="AE31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.6555111111111106E-4</v>
       </c>
       <c r="AF31">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="AH31">
+        <v>60000000</v>
+      </c>
+      <c r="AI31">
+        <v>1475115558</v>
+      </c>
       <c r="AJ31">
         <v>9</v>
       </c>
@@ -4875,11 +4985,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.2488629699476652</v>
       </c>
-    </row>
-    <row r="32" spans="1:41">
+      <c r="AP31">
+        <f>(AI32*AK31)+60000000</f>
+        <v>1671293283.175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:42">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -4971,13 +5085,19 @@
         <v>1.4216666666666664E-2</v>
       </c>
       <c r="AE32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.0211361111111104E-4</v>
       </c>
       <c r="AF32">
         <f t="shared" si="11"/>
         <v>6.0634083333333311E-6</v>
       </c>
+      <c r="AH32">
+        <v>60000000</v>
+      </c>
+      <c r="AI32">
+        <v>1571993447</v>
+      </c>
       <c r="AJ32">
         <v>10</v>
       </c>
@@ -4985,11 +5105,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.2800845441963566</v>
       </c>
-    </row>
-    <row r="33" spans="1:38">
+      <c r="AP32">
+        <f>(AI33*AK32)+60000000</f>
+        <v>1773075615.0749998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:42">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -5081,13 +5205,19 @@
         <v>2.1233333333333326E-2</v>
       </c>
       <c r="AE33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.5085444444444413E-4</v>
       </c>
       <c r="AF33">
         <f t="shared" si="11"/>
         <v>2.2632893111111098E-5</v>
       </c>
+      <c r="AH33">
+        <v>60000000</v>
+      </c>
+      <c r="AI33">
+        <v>1671293283</v>
+      </c>
       <c r="AJ33">
         <v>11</v>
       </c>
@@ -5095,11 +5225,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.3120866578012655</v>
       </c>
-    </row>
-    <row r="34" spans="1:38">
+      <c r="AP33">
+        <f>(AI34*AK33)+60000000</f>
+        <v>1877402505.3749998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:42">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -5191,13 +5325,19 @@
         <v>8.687499999999999E-3</v>
       </c>
       <c r="AE34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7.5472656249999978E-5</v>
       </c>
       <c r="AF34">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="AH34">
+        <v>60000000</v>
+      </c>
+      <c r="AI34">
+        <v>1773075615</v>
+      </c>
       <c r="AJ34">
         <v>12</v>
       </c>
@@ -5205,11 +5345,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.3448888242462971</v>
       </c>
-    </row>
-    <row r="35" spans="1:38">
+      <c r="AP34">
+        <f>(AI35*AK34)+60000000</f>
+        <v>1984337567.6249998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:42">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -5301,13 +5445,19 @@
         <v>8.9500000000000014E-3</v>
       </c>
       <c r="AE35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>8.0102500000000021E-5</v>
       </c>
       <c r="AF35">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="AH35">
+        <v>60000000</v>
+      </c>
+      <c r="AI35">
+        <v>1877402505</v>
+      </c>
       <c r="AJ35">
         <v>13</v>
       </c>
@@ -5315,11 +5465,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.3785110448524545</v>
       </c>
-    </row>
-    <row r="36" spans="1:38">
+      <c r="AP35">
+        <f>(AI36*AK35)+60000000</f>
+        <v>2093946007.1999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:42">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -5411,13 +5565,19 @@
         <v>0.18768333333333331</v>
       </c>
       <c r="AE36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.5225033611111102E-2</v>
       </c>
       <c r="AF36">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="AH36">
+        <v>60000000</v>
+      </c>
+      <c r="AI36">
+        <v>1984337568</v>
+      </c>
       <c r="AJ36">
         <v>14</v>
       </c>
@@ -5425,11 +5585,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.4129738209737657</v>
       </c>
-    </row>
-    <row r="37" spans="1:38">
+      <c r="AP36">
+        <f>(AI37*AK36)+60000000</f>
+        <v>2206294657.1749997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:42">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -5521,13 +5685,19 @@
         <v>0.2916083333333333</v>
       </c>
       <c r="AE37">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>8.5035420069444423E-2</v>
       </c>
       <c r="AF37">
         <f t="shared" si="11"/>
         <v>3.6250599575604156E-2</v>
       </c>
+      <c r="AH37">
+        <v>60000000</v>
+      </c>
+      <c r="AI37">
+        <v>2093946007</v>
+      </c>
       <c r="AJ37">
         <v>15</v>
       </c>
@@ -5535,11 +5705,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.4482981664981096</v>
       </c>
-    </row>
-    <row r="38" spans="1:38">
+      <c r="AP37">
+        <f>(AI38*AK37)+60000000</f>
+        <v>2321452023.4249997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:42">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -5631,13 +5805,19 @@
         <v>0.20651249999999999</v>
       </c>
       <c r="AE38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.2647412656249994E-2</v>
       </c>
       <c r="AF38">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="AH38">
+        <v>60000000</v>
+      </c>
+      <c r="AI38">
+        <v>2206294657</v>
+      </c>
       <c r="AJ38">
         <v>16</v>
       </c>
@@ -5645,14 +5825,110 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AL38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.4845056206605622</v>
       </c>
-    </row>
-    <row r="39" spans="1:38">
+      <c r="AP38">
+        <f>(AI39*AK38)+60000000</f>
+        <v>2439488323.5749998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:42">
       <c r="AA39" s="2">
         <f>SUM(AA23:AA38)</f>
         <v>1</v>
+      </c>
+      <c r="AH39">
+        <v>60000000</v>
+      </c>
+      <c r="AI39">
+        <v>2321452023</v>
+      </c>
+      <c r="AJ39">
+        <v>17</v>
+      </c>
+      <c r="AK39">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="AL39">
+        <f t="shared" si="12"/>
+        <v>1.5216182611770761</v>
+      </c>
+      <c r="AP39">
+        <f>(AI40*AK39)+60000000</f>
+        <v>2560475532.0999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:42">
+      <c r="AH40">
+        <v>60000000</v>
+      </c>
+      <c r="AI40">
+        <v>2439488324</v>
+      </c>
+      <c r="AJ40">
+        <v>18</v>
+      </c>
+      <c r="AK40">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="AL40">
+        <f t="shared" si="12"/>
+        <v>1.5596587177065029</v>
+      </c>
+      <c r="AP40">
+        <f>(AI41*AK40)+60000000</f>
+        <v>2684487420.2999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:42">
+      <c r="AH41">
+        <v>60000000</v>
+      </c>
+      <c r="AI41">
+        <v>2560475532</v>
+      </c>
+      <c r="AJ41">
+        <v>19</v>
+      </c>
+      <c r="AK41">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="AL41">
+        <f t="shared" si="12"/>
+        <v>1.5986501856491653</v>
+      </c>
+      <c r="AP41">
+        <f>(AI42*AK41)+60000000</f>
+        <v>2811599605.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:42">
+      <c r="AH42">
+        <v>60000000</v>
+      </c>
+      <c r="AI42">
+        <v>2684487420</v>
+      </c>
+      <c r="AJ42">
+        <v>20</v>
+      </c>
+      <c r="AK42">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="AL42">
+        <f t="shared" si="12"/>
+        <v>1.6386164402903942</v>
+      </c>
+    </row>
+    <row r="43" spans="1:42">
+      <c r="AK43">
+        <v>1.0249999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:42">
+      <c r="AH44" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>